<commit_message>
utilizando densidade populacional para classificar grandes cidades
</commit_message>
<xml_diff>
--- a/output/flourish_municipios_200mil.xlsx
+++ b/output/flourish_municipios_200mil.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>ideologia</t>
   </si>
@@ -97,19 +97,13 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Centro Dem</t>
+    <t>Centro</t>
   </si>
   <si>
     <t>Direita</t>
   </si>
   <si>
     <t>Esquerda</t>
-  </si>
-  <si>
-    <t>Extinto</t>
-  </si>
-  <si>
-    <t>Centrao</t>
   </si>
 </sst>
 </file>
@@ -539,10 +533,10 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -568,7 +562,7 @@
         <v>30</v>
       </c>
       <c r="F4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>28</v>
@@ -660,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -712,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -738,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -790,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -799,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
         <v>8</v>
-      </c>
-      <c r="F13">
-        <v>9</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -816,7 +810,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -906,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -1024,7 +1018,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -1128,7 +1122,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>0</v>

</xml_diff>